<commit_message>
Se incluyen algunos logs.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>Results.xlsx</t>
+  </si>
+  <si>
+    <t>Cantidad de reintentos</t>
+  </si>
+  <si>
+    <t>Retry</t>
   </si>
 </sst>
 </file>
@@ -332,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -350,6 +356,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -667,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -738,10 +747,10 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -855,64 +864,74 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="6"/>
+      <c r="A15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="11">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="A16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="6"/>
+      <c r="A18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="A19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1880,11 +1899,12 @@
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1896,7 +1916,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>